<commit_message>
Updated to .NET 7.0
</commit_message>
<xml_diff>
--- a/Test techniques assignment 1.xlsx
+++ b/Test techniques assignment 1.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hk/Documents/Undervisning/Test Autumn 2018/Solutions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hk/Documents/Undervisning/Test/Solutions/Test-techniques-assignment-1-Solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE073403-88F7-994D-9FA4-173D3581F2A5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C20071F-6D77-6B4C-B5F9-AFC87B14F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="13160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -485,7 +495,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>